<commit_message>
All assertions completed as Webtest includes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Testcase Name</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>hf_challenge_1578856393166@hf393166.com</t>
+  </si>
+  <si>
+    <t>hf_challenge_1578859292589@hf292589.com</t>
+  </si>
+  <si>
+    <t>hf_challenge_1578859334762@hf334762.com</t>
+  </si>
+  <si>
+    <t>hf_challenge_1578861964734@hf964734.com</t>
+  </si>
+  <si>
+    <t>hf_challenge_1578862413072@hf413072.com</t>
   </si>
 </sst>
 </file>
@@ -408,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Take screenshot is added Constants class is added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D868D861-2F41-4E76-95F5-3DB28B7BC3F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA1865D-8C96-42B2-BC48-5EA4439FD1D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1752" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="3705" windowWidth="18210" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="SigninData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Testcase Name</t>
   </si>
@@ -49,41 +50,61 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>hf_challenge_1578855297299@hf297299.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578856393166@hf393166.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578859292589@hf292589.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578859334762@hf334762.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578861964734@hf964734.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578862413072@hf413072.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578864948662@hf948662.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578866206494@hf206494.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578867073428@hf073428.com</t>
-  </si>
-  <si>
-    <t>hf_challenge_1578867238804@hf238804.com</t>
+    <t>hf_challenge_1578909836186@hf836186.com</t>
+  </si>
+  <si>
+    <t>useremail</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Id_state</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Phone_mobile</t>
+  </si>
+  <si>
+    <t>Alias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,17 +427,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,18 +448,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -449,7 +470,7 @@
         <v>111111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -458,6 +479,84 @@
       </c>
       <c r="C4" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LUnrestricted </oddFooter>
+    <evenFooter xml:space="preserve">&amp;LUnrestricted </evenFooter>
+    <firstFooter xml:space="preserve">&amp;LUnrestricted </firstFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED81F245-3C41-47B2-9313-A0E1EF5E3677}">
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>